<commit_message>
Added supervisor field to excel template for uploading report info.
The field was already implemented in the import function - no changes needed.
</commit_message>
<xml_diff>
--- a/find_artek/static/publications/docs/ARTEK_report_list.xlsx
+++ b/find_artek/static/publications/docs/ARTEK_report_list.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="20940" windowHeight="10365"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="20940" windowHeight="10380"/>
   </bookViews>
   <sheets>
     <sheet name="ARTEK rapporter" sheetId="1" r:id="rId1"/>
@@ -70,12 +70,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thomas Ingeman-Nielsen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+List of supervisors separated by commas:
+First Middle Last, First Middle Last, ...</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>number</t>
   </si>
@@ -88,12 +113,15 @@
   <si>
     <t>author</t>
   </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +293,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -299,6 +328,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -474,23 +504,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="104" style="3" customWidth="1"/>
     <col min="3" max="3" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="157.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -503,9 +534,12 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection password="CC3D" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>"Infrastruktur,Byggeri,Miljø,Energi,Geoteknik,Råstoffer,Samfund"</formula1>

</xml_diff>

<commit_message>
Added supervisor field support to xlsx publication import.
Also updated the xlsx template.
</commit_message>
<xml_diff>
--- a/find_artek/static/publications/docs/ARTEK_report_list.xlsx
+++ b/find_artek/static/publications/docs/ARTEK_report_list.xlsx
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>number</t>
   </si>
@@ -114,7 +114,10 @@
     <t>author</t>
   </si>
   <si>
-    <t>Supervisor</t>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -192,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
@@ -204,6 +207,13 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,23 +515,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="104" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="157.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="85.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="39.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -529,20 +540,29 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="5"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C1048576">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Infrastruktur,Byggeri,Miljø,Energi,Geoteknik,Råstoffer,Samfund"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
+      <formula1>"STUDENTREPORT, ARTICLE, MASTERSTHESIS, BOOK, MANUAL, UNPUBLISHED, CONFERENCE  PROCEEDINGS, INBOOK, INPROCEEDINGS, PHDTHESIS, TECHREPORT"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
UPDATED: report list Excel template updated with better column descriptions.
</commit_message>
<xml_diff>
--- a/find_artek/static/publications/docs/ARTEK_report_list.xlsx
+++ b/find_artek/static/publications/docs/ARTEK_report_list.xlsx
@@ -41,7 +41,7 @@
           <t xml:space="preserve">
 Report number has the format:
 XX-YY
-where XX is the year and YY is a two digit integer.</t>
+where XX is the two digit year and YY is a two digit integer.</t>
         </r>
       </text>
     </comment>
@@ -65,8 +65,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-List of authors separated by commas:
-First Middle Last, First Middle Last, ...</t>
+List of authors separated by semicolon (or comma):
+First Middle Last; First Middle Last; …
+May also contain studynumbers of students:
+s140001; s121005;...
+</t>
         </r>
       </text>
     </comment>
@@ -90,8 +93,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-List of supervisors separated by commas:
-First Middle Last, First Middle Last, ...</t>
+List of supervisors separated by semicolon (or comma):
+First Middle Last; First Middle Last; …
+May also contain official DTU initials of employees:
+thin; gunki; …
+Or it can be a combination of names and initials (e.g. if external supervisor):
+sabol; Lis Bach</t>
         </r>
       </text>
     </comment>
@@ -515,11 +522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,9 +559,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F2" s="5"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <dataValidations count="2">

</xml_diff>